<commit_message>
Deploying to gh-pages from  @ 44b225e0132bfbfa9cc91f6030fa1d153fb037f8 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_4-3-1.xlsx
+++ b/assets/excel/2021_4-3-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BiesterChristophLSN\Desktop\_Schrott\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7104700A-FC26-42FE-A9BF-29F784AA3634}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D6241C7-595F-4170-B937-2970C18E28D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{20965728-CEF5-43F8-82AF-E84F8D6D6224}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8688" xr2:uid="{20965728-CEF5-43F8-82AF-E84F8D6D6224}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -412,6 +412,9 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -445,9 +448,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -768,52 +768,52 @@
   <dimension ref="B1:M109"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B9"/>
+      <selection activeCell="J7" sqref="J7:L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-    </row>
-    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -826,56 +826,56 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+    <row r="6" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="19"/>
-    </row>
-    <row r="7" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="26" t="s">
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="20"/>
+    </row>
+    <row r="7" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="25"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="19"/>
-    </row>
-    <row r="8" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="20"/>
+    </row>
+    <row r="8" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="25"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
@@ -895,57 +895,57 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="25"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="20" t="s">
+    <row r="9" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="26"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="19"/>
-    </row>
-    <row r="10" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="29">
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="20"/>
+    </row>
+    <row r="10" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="18">
         <v>1</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="18">
         <v>2</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="18">
         <v>3</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="18">
         <v>4</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="18">
         <v>5</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="18">
         <v>6</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="18">
         <v>7</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="18">
         <v>8</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="18">
         <v>9</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="18">
         <v>10</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="18">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
@@ -981,7 +981,7 @@
       </c>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>36</v>
       </c>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>37</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
         <v>38</v>
       </c>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="16" t="s">
         <v>39</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
         <v>34</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>35</v>
       </c>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="14" t="s">
         <v>36</v>
       </c>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
         <v>37</v>
       </c>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
         <v>38</v>
       </c>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="16" t="s">
         <v>39</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="14" t="s">
         <v>34</v>
       </c>
@@ -1411,7 +1411,7 @@
       </c>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
         <v>35</v>
       </c>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
         <v>36</v>
       </c>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
         <v>37</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
         <v>38</v>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="16" t="s">
         <v>39</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>34</v>
       </c>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="14" t="s">
         <v>35</v>
       </c>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>36</v>
       </c>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="14" t="s">
         <v>37</v>
       </c>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
         <v>38</v>
       </c>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="16" t="s">
         <v>39</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
         <v>34</v>
       </c>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="14" t="s">
         <v>35</v>
       </c>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="M36" s="7"/>
     </row>
-    <row r="37" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="14" t="s">
         <v>36</v>
       </c>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="14" t="s">
         <v>37</v>
       </c>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="14" t="s">
         <v>38</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="16" t="s">
         <v>39</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="41" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="14" t="s">
         <v>34</v>
       </c>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="M41" s="7"/>
     </row>
-    <row r="42" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="14" t="s">
         <v>35</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="14" t="s">
         <v>36</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="14" t="s">
         <v>37</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="14" t="s">
         <v>38</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="16" t="s">
         <v>39</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="47" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="14" t="s">
         <v>34</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="14" t="s">
         <v>35</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="49" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="14" t="s">
         <v>36</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="14" t="s">
         <v>37</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="14" t="s">
         <v>38</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="16" t="s">
         <v>39</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>1563</v>
       </c>
     </row>
-    <row r="53" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="14" t="s">
         <v>34</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="14" t="s">
         <v>35</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="55" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="14" t="s">
         <v>36</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="14" t="s">
         <v>37</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="14" t="s">
         <v>38</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="16" t="s">
         <v>39</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="59" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="14" t="s">
         <v>34</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="14" t="s">
         <v>35</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="61" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="14" t="s">
         <v>36</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="14" t="s">
         <v>37</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="14" t="s">
         <v>38</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="16" t="s">
         <v>39</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="65" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="14" t="s">
         <v>34</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="14" t="s">
         <v>35</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="67" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="14" t="s">
         <v>36</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="14" t="s">
         <v>37</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="14" t="s">
         <v>38</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="16" t="s">
         <v>39</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="71" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="14" t="s">
         <v>34</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="14" t="s">
         <v>35</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="73" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="14" t="s">
         <v>36</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="14" t="s">
         <v>37</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="14" t="s">
         <v>38</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="16" t="s">
         <v>39</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="77" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="14" t="s">
         <v>34</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="14" t="s">
         <v>35</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="79" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="14" t="s">
         <v>36</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="14" t="s">
         <v>37</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="14" t="s">
         <v>38</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="16" t="s">
         <v>39</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>2305</v>
       </c>
     </row>
-    <row r="83" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="14" t="s">
         <v>34</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="14" t="s">
         <v>35</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="85" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="14" t="s">
         <v>36</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="14" t="s">
         <v>37</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="14" t="s">
         <v>38</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="16" t="s">
         <v>39</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>2284</v>
       </c>
     </row>
-    <row r="89" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="14" t="s">
         <v>34</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="90" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="14" t="s">
         <v>35</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="91" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="14" t="s">
         <v>36</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="14" t="s">
         <v>37</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="14" t="s">
         <v>38</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="94" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="16" t="s">
         <v>39</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="95" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="14" t="s">
         <v>34</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="14" t="s">
         <v>35</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="97" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="14" t="s">
         <v>36</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="14" t="s">
         <v>37</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="14" t="s">
         <v>38</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="16" t="s">
         <v>39</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="101" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="8"/>
       <c r="C101" s="9"/>
       <c r="D101" s="10"/>
@@ -4134,7 +4134,7 @@
       <c r="K101" s="10"/>
       <c r="L101" s="10"/>
     </row>
-    <row r="102" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="11" t="s">
         <v>27</v>
       </c>
@@ -4149,7 +4149,7 @@
       <c r="K102" s="11"/>
       <c r="L102" s="11"/>
     </row>
-    <row r="103" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
@@ -4161,7 +4161,7 @@
       <c r="K103" s="11"/>
       <c r="L103" s="11"/>
     </row>
-    <row r="104" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="11" t="s">
         <v>28</v>
       </c>
@@ -4176,23 +4176,23 @@
       <c r="K104" s="11"/>
       <c r="L104" s="11"/>
     </row>
-    <row r="105" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="12" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ a50c71b5d402a91eb434de31ad2bfd4605199aff 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_4-3-1.xlsx
+++ b/assets/excel/2021_4-3-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BiesterChristophLSN\Desktop\_Schrott\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D6241C7-595F-4170-B937-2970C18E28D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{565B25C1-8E08-4191-BB0F-0B81D3641725}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8688" xr2:uid="{20965728-CEF5-43F8-82AF-E84F8D6D6224}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{20965728-CEF5-43F8-82AF-E84F8D6D6224}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="43">
   <si>
     <t>Indikator 4.3.1: Ausländische Studentinnen und Studenten nach Land des Erwerbs der Studienberechtigung</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>Staaten insgesamt</t>
+  </si>
+  <si>
+    <t>WS 2020/21</t>
+  </si>
+  <si>
+    <t>Syrien Arab. Republik</t>
+  </si>
+  <si>
+    <t>Iran Islamische Republik</t>
   </si>
 </sst>
 </file>
@@ -765,25 +774,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92371CE9-FDE3-4655-96C5-EAAB9E96F280}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:M109"/>
+  <dimension ref="B1:M115"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:L7"/>
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
@@ -798,7 +807,7 @@
       <c r="K3" s="22"/>
       <c r="L3" s="22"/>
     </row>
-    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
@@ -813,7 +822,7 @@
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -826,7 +835,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>2</v>
       </c>
@@ -847,7 +856,7 @@
       <c r="K6" s="19"/>
       <c r="L6" s="20"/>
     </row>
-    <row r="7" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="25"/>
       <c r="C7" s="28"/>
       <c r="D7" s="27" t="s">
@@ -870,7 +879,7 @@
       <c r="K7" s="19"/>
       <c r="L7" s="20"/>
     </row>
-    <row r="8" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="25"/>
       <c r="C8" s="28"/>
       <c r="D8" s="29"/>
@@ -895,7 +904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="29"/>
       <c r="D9" s="21" t="s">
@@ -910,7 +919,7 @@
       <c r="K9" s="19"/>
       <c r="L9" s="20"/>
     </row>
-    <row r="10" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18">
         <v>1</v>
       </c>
@@ -945,7 +954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
@@ -981,7 +990,7 @@
       </c>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +1026,7 @@
       </c>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>36</v>
       </c>
@@ -1053,7 +1062,7 @@
       </c>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>37</v>
       </c>
@@ -1089,7 +1098,7 @@
       </c>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>38</v>
       </c>
@@ -1125,7 +1134,7 @@
       </c>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
         <v>39</v>
       </c>
@@ -1160,7 +1169,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>34</v>
       </c>
@@ -1196,7 +1205,7 @@
       </c>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>35</v>
       </c>
@@ -1232,7 +1241,7 @@
       </c>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>36</v>
       </c>
@@ -1268,7 +1277,7 @@
       </c>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>37</v>
       </c>
@@ -1304,7 +1313,7 @@
       </c>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>38</v>
       </c>
@@ -1340,7 +1349,7 @@
       </c>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
         <v>39</v>
       </c>
@@ -1375,7 +1384,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
         <v>34</v>
       </c>
@@ -1411,7 +1420,7 @@
       </c>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
         <v>35</v>
       </c>
@@ -1447,7 +1456,7 @@
       </c>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
         <v>36</v>
       </c>
@@ -1483,7 +1492,7 @@
       </c>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
         <v>37</v>
       </c>
@@ -1519,7 +1528,7 @@
       </c>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
         <v>38</v>
       </c>
@@ -1555,7 +1564,7 @@
       </c>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
         <v>39</v>
       </c>
@@ -1590,7 +1599,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>34</v>
       </c>
@@ -1626,7 +1635,7 @@
       </c>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>35</v>
       </c>
@@ -1662,7 +1671,7 @@
       </c>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>36</v>
       </c>
@@ -1698,7 +1707,7 @@
       </c>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>37</v>
       </c>
@@ -1734,7 +1743,7 @@
       </c>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
         <v>38</v>
       </c>
@@ -1770,7 +1779,7 @@
       </c>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="16" t="s">
         <v>39</v>
       </c>
@@ -1805,7 +1814,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
         <v>34</v>
       </c>
@@ -1841,7 +1850,7 @@
       </c>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
         <v>35</v>
       </c>
@@ -1877,7 +1886,7 @@
       </c>
       <c r="M36" s="7"/>
     </row>
-    <row r="37" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
         <v>36</v>
       </c>
@@ -1913,7 +1922,7 @@
       </c>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
         <v>37</v>
       </c>
@@ -1949,7 +1958,7 @@
       </c>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
         <v>38</v>
       </c>
@@ -1985,7 +1994,7 @@
       </c>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="16" t="s">
         <v>39</v>
       </c>
@@ -2020,7 +2029,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="41" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" s="6" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
         <v>34</v>
       </c>
@@ -2056,7 +2065,7 @@
       </c>
       <c r="M41" s="7"/>
     </row>
-    <row r="42" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
         <v>35</v>
       </c>
@@ -2091,7 +2100,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
         <v>36</v>
       </c>
@@ -2126,7 +2135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
         <v>37</v>
       </c>
@@ -2161,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
         <v>38</v>
       </c>
@@ -2196,7 +2205,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="16" t="s">
         <v>39</v>
       </c>
@@ -2231,7 +2240,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="47" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
         <v>34</v>
       </c>
@@ -2266,7 +2275,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
         <v>35</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="49" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
         <v>36</v>
       </c>
@@ -2336,7 +2345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="14" t="s">
         <v>37</v>
       </c>
@@ -2371,7 +2380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
         <v>38</v>
       </c>
@@ -2406,7 +2415,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="16" t="s">
         <v>39</v>
       </c>
@@ -2441,7 +2450,7 @@
         <v>1563</v>
       </c>
     </row>
-    <row r="53" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
         <v>34</v>
       </c>
@@ -2476,7 +2485,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="14" t="s">
         <v>35</v>
       </c>
@@ -2511,7 +2520,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="55" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
         <v>36</v>
       </c>
@@ -2546,7 +2555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="14" t="s">
         <v>37</v>
       </c>
@@ -2581,7 +2590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
         <v>38</v>
       </c>
@@ -2616,7 +2625,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="16" t="s">
         <v>39</v>
       </c>
@@ -2651,7 +2660,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="59" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
         <v>34</v>
       </c>
@@ -2686,7 +2695,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
         <v>35</v>
       </c>
@@ -2721,7 +2730,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="61" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
         <v>36</v>
       </c>
@@ -2756,7 +2765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
         <v>37</v>
       </c>
@@ -2791,7 +2800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="14" t="s">
         <v>38</v>
       </c>
@@ -2826,7 +2835,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="s">
         <v>39</v>
       </c>
@@ -2861,7 +2870,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="65" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
         <v>34</v>
       </c>
@@ -2896,7 +2905,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="14" t="s">
         <v>35</v>
       </c>
@@ -2931,7 +2940,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="67" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="14" t="s">
         <v>36</v>
       </c>
@@ -2966,7 +2975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="14" t="s">
         <v>37</v>
       </c>
@@ -3001,7 +3010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="14" t="s">
         <v>38</v>
       </c>
@@ -3036,7 +3045,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="16" t="s">
         <v>39</v>
       </c>
@@ -3071,7 +3080,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="71" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="14" t="s">
         <v>34</v>
       </c>
@@ -3106,7 +3115,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="14" t="s">
         <v>35</v>
       </c>
@@ -3141,7 +3150,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="73" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="14" t="s">
         <v>36</v>
       </c>
@@ -3176,7 +3185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
         <v>37</v>
       </c>
@@ -3211,7 +3220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="14" t="s">
         <v>38</v>
       </c>
@@ -3246,7 +3255,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
         <v>39</v>
       </c>
@@ -3281,7 +3290,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="77" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="14" t="s">
         <v>34</v>
       </c>
@@ -3316,7 +3325,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="14" t="s">
         <v>35</v>
       </c>
@@ -3351,7 +3360,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="79" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="14" t="s">
         <v>36</v>
       </c>
@@ -3386,7 +3395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
         <v>37</v>
       </c>
@@ -3421,7 +3430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="14" t="s">
         <v>38</v>
       </c>
@@ -3456,7 +3465,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="16" t="s">
         <v>39</v>
       </c>
@@ -3491,7 +3500,7 @@
         <v>2305</v>
       </c>
     </row>
-    <row r="83" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="14" t="s">
         <v>34</v>
       </c>
@@ -3526,7 +3535,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
         <v>35</v>
       </c>
@@ -3561,7 +3570,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="85" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
         <v>36</v>
       </c>
@@ -3596,7 +3605,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="14" t="s">
         <v>37</v>
       </c>
@@ -3631,7 +3640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="14" t="s">
         <v>38</v>
       </c>
@@ -3666,7 +3675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="16" t="s">
         <v>39</v>
       </c>
@@ -3701,7 +3710,7 @@
         <v>2284</v>
       </c>
     </row>
-    <row r="89" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
         <v>34</v>
       </c>
@@ -3736,7 +3745,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="90" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="14" t="s">
         <v>35</v>
       </c>
@@ -3771,7 +3780,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="91" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="14" t="s">
         <v>36</v>
       </c>
@@ -3806,7 +3815,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="14" t="s">
         <v>37</v>
       </c>
@@ -3841,7 +3850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
         <v>38</v>
       </c>
@@ -3876,7 +3885,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="94" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="16" t="s">
         <v>39</v>
       </c>
@@ -3911,7 +3920,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="95" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="14" t="s">
         <v>34</v>
       </c>
@@ -3946,7 +3955,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="14" t="s">
         <v>35</v>
       </c>
@@ -3981,7 +3990,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="97" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="14" t="s">
         <v>36</v>
       </c>
@@ -4016,7 +4025,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="14" t="s">
         <v>37</v>
       </c>
@@ -4051,7 +4060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="14" t="s">
         <v>38</v>
       </c>
@@ -4086,7 +4095,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="16" t="s">
         <v>39</v>
       </c>
@@ -4121,79 +4130,289 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="101" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="8"/>
-      <c r="C101" s="9"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="10"/>
-      <c r="F101" s="10"/>
-      <c r="G101" s="10"/>
-      <c r="H101" s="10"/>
-      <c r="I101" s="10"/>
-      <c r="J101" s="10"/>
-      <c r="K101" s="10"/>
-      <c r="L101" s="10"/>
-    </row>
-    <row r="102" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="11" t="s">
+    <row r="101" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C101" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D101" s="15">
+        <v>4286</v>
+      </c>
+      <c r="E101" s="15">
+        <v>2523</v>
+      </c>
+      <c r="F101" s="15">
+        <v>1763</v>
+      </c>
+      <c r="G101" s="15">
+        <v>4157</v>
+      </c>
+      <c r="H101" s="15">
+        <v>2451</v>
+      </c>
+      <c r="I101" s="15">
+        <v>1706</v>
+      </c>
+      <c r="J101" s="15">
+        <v>129</v>
+      </c>
+      <c r="K101" s="15">
+        <v>72</v>
+      </c>
+      <c r="L101" s="15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D102" s="15">
+        <v>1919</v>
+      </c>
+      <c r="E102" s="15">
+        <v>979</v>
+      </c>
+      <c r="F102" s="15">
+        <v>940</v>
+      </c>
+      <c r="G102" s="15">
+        <v>518</v>
+      </c>
+      <c r="H102" s="15">
+        <v>310</v>
+      </c>
+      <c r="I102" s="15">
+        <v>208</v>
+      </c>
+      <c r="J102" s="15">
+        <v>1401</v>
+      </c>
+      <c r="K102" s="15">
+        <v>669</v>
+      </c>
+      <c r="L102" s="15">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D103" s="15">
+        <v>1751</v>
+      </c>
+      <c r="E103" s="15">
+        <v>1336</v>
+      </c>
+      <c r="F103" s="15">
+        <v>415</v>
+      </c>
+      <c r="G103" s="15">
+        <v>1528</v>
+      </c>
+      <c r="H103" s="15">
+        <v>1199</v>
+      </c>
+      <c r="I103" s="15">
+        <v>329</v>
+      </c>
+      <c r="J103" s="15">
+        <v>223</v>
+      </c>
+      <c r="K103" s="15">
+        <v>137</v>
+      </c>
+      <c r="L103" s="15">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="104" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D104" s="15">
+        <v>1502</v>
+      </c>
+      <c r="E104" s="15">
+        <v>1080</v>
+      </c>
+      <c r="F104" s="15">
+        <v>422</v>
+      </c>
+      <c r="G104" s="15">
+        <v>1493</v>
+      </c>
+      <c r="H104" s="15">
+        <v>1074</v>
+      </c>
+      <c r="I104" s="15">
+        <v>419</v>
+      </c>
+      <c r="J104" s="15">
+        <v>9</v>
+      </c>
+      <c r="K104" s="15">
+        <v>6</v>
+      </c>
+      <c r="L104" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C105" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D105" s="15">
+        <v>1124</v>
+      </c>
+      <c r="E105" s="15">
+        <v>586</v>
+      </c>
+      <c r="F105" s="15">
+        <v>538</v>
+      </c>
+      <c r="G105" s="15">
+        <v>1062</v>
+      </c>
+      <c r="H105" s="15">
+        <v>554</v>
+      </c>
+      <c r="I105" s="15">
+        <v>508</v>
+      </c>
+      <c r="J105" s="15">
+        <v>62</v>
+      </c>
+      <c r="K105" s="15">
+        <v>32</v>
+      </c>
+      <c r="L105" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="106" spans="2:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C106" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D106" s="17">
+        <v>25111</v>
+      </c>
+      <c r="E106" s="17">
+        <v>14481</v>
+      </c>
+      <c r="F106" s="17">
+        <v>10630</v>
+      </c>
+      <c r="G106" s="17">
+        <v>20647</v>
+      </c>
+      <c r="H106" s="17">
+        <v>12329</v>
+      </c>
+      <c r="I106" s="17">
+        <v>8318</v>
+      </c>
+      <c r="J106" s="17">
+        <v>4464</v>
+      </c>
+      <c r="K106" s="17">
+        <v>2152</v>
+      </c>
+      <c r="L106" s="17">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="107" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="8"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="10"/>
+      <c r="L107" s="10"/>
+    </row>
+    <row r="108" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
-      <c r="I102" s="11"/>
-      <c r="J102" s="11"/>
-      <c r="K102" s="11"/>
-      <c r="L102" s="11"/>
-    </row>
-    <row r="103" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="11"/>
-      <c r="K103" s="11"/>
-      <c r="L103" s="11"/>
-    </row>
-    <row r="104" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="11" t="s">
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="11"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="11"/>
+      <c r="K108" s="11"/>
+      <c r="L108" s="11"/>
+    </row>
+    <row r="109" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
+      <c r="G109" s="11"/>
+      <c r="H109" s="11"/>
+      <c r="I109" s="11"/>
+      <c r="J109" s="11"/>
+      <c r="K109" s="11"/>
+      <c r="L109" s="11"/>
+    </row>
+    <row r="110" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
-      <c r="G104" s="11"/>
-      <c r="H104" s="11"/>
-      <c r="I104" s="11"/>
-      <c r="J104" s="11"/>
-      <c r="K104" s="11"/>
-      <c r="L104" s="11"/>
-    </row>
-    <row r="105" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="11" t="s">
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="11"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="11"/>
+      <c r="I110" s="11"/>
+      <c r="J110" s="11"/>
+      <c r="K110" s="11"/>
+      <c r="L110" s="11"/>
+    </row>
+    <row r="111" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="11" t="s">
+    <row r="113" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="11" t="s">
+    <row r="114" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="12" t="s">
+    <row r="115" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="12" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4213,7 +4432,7 @@
     <mergeCell ref="G7:I7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B109" r:id="rId1" xr:uid="{2442C1A8-2977-4FA5-B5F8-D802121BC484}"/>
+    <hyperlink ref="B115" r:id="rId1" xr:uid="{2442C1A8-2977-4FA5-B5F8-D802121BC484}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>